<commit_message>
Stage 5/5: Rabin-Karp problems...
</commit_message>
<xml_diff>
--- a/File Type Analyzer/Docs/RK.xlsx
+++ b/File Type Analyzer/Docs/RK.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -60,7 +61,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,13 +79,26 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -96,10 +110,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -109,9 +124,12 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Хороший" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -389,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,10 +423,12 @@
     <col min="9" max="9" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="16.28515625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -437,7 +457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -452,6 +472,9 @@
       </c>
       <c r="E2" s="1">
         <v>1000000009</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
       </c>
       <c r="G2" t="s">
         <v>0</v>
@@ -472,7 +495,7 @@
         <f>H2*C2</f>
         <v>33</v>
       </c>
-      <c r="L2" s="1">
+      <c r="L2" s="6">
         <f>MOD(L1+M2,$E$2)</f>
         <v>33</v>
       </c>
@@ -481,7 +504,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -493,6 +516,9 @@
         <f>MOD(C2*$D$2,$E$2)</f>
         <v>53</v>
       </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
       <c r="G3" t="s">
         <v>1</v>
       </c>
@@ -512,7 +538,7 @@
         <f>K2+H3*C3</f>
         <v>1835</v>
       </c>
-      <c r="L3" s="1">
+      <c r="L3" s="6">
         <f t="shared" ref="L3:L9" si="3">MOD(L2+M3,$E$2)</f>
         <v>1835</v>
       </c>
@@ -521,7 +547,7 @@
         <v>1802</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -533,6 +559,9 @@
         <f t="shared" ref="C4:C15" si="6">MOD(C3*$D$2,$E$2)</f>
         <v>2809</v>
       </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
       <c r="G4" t="s">
         <v>0</v>
       </c>
@@ -552,7 +581,7 @@
         <f t="shared" ref="K4:K9" si="7">K3+H4*C4</f>
         <v>94532</v>
       </c>
-      <c r="L4" s="1">
+      <c r="L4" s="6">
         <f t="shared" si="3"/>
         <v>94532</v>
       </c>
@@ -561,7 +590,7 @@
         <v>92697</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -573,6 +602,9 @@
         <f t="shared" si="6"/>
         <v>148877</v>
       </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
       <c r="G5" t="s">
         <v>2</v>
       </c>
@@ -592,7 +624,7 @@
         <f t="shared" si="7"/>
         <v>5305227</v>
       </c>
-      <c r="L5" s="1">
+      <c r="L5" s="6">
         <f t="shared" si="3"/>
         <v>5305227</v>
       </c>
@@ -601,7 +633,7 @@
         <v>5210695</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -613,6 +645,9 @@
         <f t="shared" si="6"/>
         <v>7890481</v>
       </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
       <c r="G6" t="s">
         <v>0</v>
       </c>
@@ -632,7 +667,7 @@
         <f t="shared" si="7"/>
         <v>265691100</v>
       </c>
-      <c r="L6" s="1">
+      <c r="L6" s="6">
         <f t="shared" si="3"/>
         <v>265691100</v>
       </c>
@@ -641,7 +676,7 @@
         <v>260385873</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -653,6 +688,9 @@
         <f t="shared" si="6"/>
         <v>418195493</v>
       </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
       <c r="G7" t="s">
         <v>1</v>
       </c>
@@ -672,7 +710,7 @@
         <f t="shared" si="7"/>
         <v>14484337862</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L7" s="6">
         <f t="shared" si="3"/>
         <v>484337736</v>
       </c>
@@ -681,7 +719,7 @@
         <v>218646636</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -693,6 +731,9 @@
         <f t="shared" si="6"/>
         <v>164360931</v>
       </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
       <c r="G8" t="s">
         <v>0</v>
       </c>
@@ -712,7 +753,7 @@
         <f t="shared" si="7"/>
         <v>19908248585</v>
       </c>
-      <c r="L8" s="1">
+      <c r="L8" s="6">
         <f t="shared" si="3"/>
         <v>908248414</v>
       </c>
@@ -721,7 +762,7 @@
         <v>423910678</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -733,6 +774,9 @@
         <f t="shared" si="6"/>
         <v>711129271</v>
       </c>
+      <c r="F9">
+        <v>7</v>
+      </c>
       <c r="G9" t="s">
         <v>3</v>
       </c>
@@ -752,7 +796,7 @@
         <f t="shared" si="7"/>
         <v>45508902341</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L9" s="6">
         <f t="shared" si="3"/>
         <v>508901936</v>
       </c>
@@ -761,7 +805,7 @@
         <v>600653531</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -774,7 +818,7 @@
         <v>689851030</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -794,22 +838,22 @@
       </c>
       <c r="I11" s="4" t="str">
         <f>"hp(0:"&amp;H12&amp;")"</f>
-        <v>hp(0:6)</v>
+        <v>hp(0:2)</v>
       </c>
       <c r="J11" s="4" t="str">
         <f>"hp(0:"&amp;G12&amp;")"</f>
-        <v>hp(0:5)</v>
-      </c>
-      <c r="K11" s="1" t="str">
+        <v>hp(0:0)</v>
+      </c>
+      <c r="K11" s="4" t="str">
         <f>I11&amp;"-"&amp;J11</f>
-        <v>hp(0:6)-hp(0:5)</v>
+        <v>hp(0:2)-hp(0:0)</v>
       </c>
       <c r="L11" s="4" t="str">
         <f>"a^"&amp;G12</f>
-        <v>a^5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+        <v>a^0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -822,33 +866,33 @@
         <v>791525837</v>
       </c>
       <c r="G12">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H12">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I12" s="1">
         <f>INDEX(L1:L9,H12+1)</f>
-        <v>484337736</v>
+        <v>1835</v>
       </c>
       <c r="J12" s="1">
         <f>INDEX(L1:L9,G12+1)</f>
-        <v>265691100</v>
+        <v>0</v>
       </c>
       <c r="K12" s="1">
         <f>I12-J12</f>
-        <v>218646636</v>
+        <v>1835</v>
       </c>
       <c r="L12" s="1">
         <f>INDEX(C:C,G12+2)</f>
-        <v>418195493</v>
+        <v>1</v>
       </c>
       <c r="M12" s="2">
-        <f>K12/L12</f>
-        <v>0.52283355430614364</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+        <f>MOD(K12*L12,E2)</f>
+        <v>1835</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -861,7 +905,7 @@
         <v>950868992</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -873,8 +917,14 @@
         <f t="shared" si="6"/>
         <v>396056126</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O14">
+        <v>1835</v>
+      </c>
+      <c r="P14" s="1">
+        <v>479032509</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -885,6 +935,73 @@
       <c r="C15" s="1">
         <f t="shared" si="6"/>
         <v>990974498</v>
+      </c>
+      <c r="O15">
+        <f>O14*C6</f>
+        <v>14479032635</v>
+      </c>
+      <c r="P15">
+        <f>P14/L12</f>
+        <v>479032509</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A1:A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1835</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>94532</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>5305227</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>265691100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>484337736</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>908248414</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>508901936</v>
       </c>
     </row>
   </sheetData>

</xml_diff>